<commit_message>
ESP8266 DEEP SLEEP TEORIE
</commit_message>
<xml_diff>
--- a/Mereni/Výsledky měření.xlsx
+++ b/Mereni/Výsledky měření.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiricek.milan01\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming\MP_NETIO_BUTTON\Mereni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136949F8-C9FC-40E5-A928-FA58ABC79FFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB55D663-74DC-4F54-B554-D9D2815B0B38}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11C4E342-A7A8-4CD3-AA61-06B44577753C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{11C4E342-A7A8-4CD3-AA61-06B44577753C}"/>
   </bookViews>
   <sheets>
-    <sheet name="HTTP Komunikace" sheetId="2" r:id="rId1"/>
-    <sheet name="Dynamické WiFi" sheetId="3" r:id="rId2"/>
-    <sheet name="Statické WiFi" sheetId="5" r:id="rId3"/>
-    <sheet name="Zabezpečení" sheetId="6" r:id="rId4"/>
+    <sheet name="Reakce režimů" sheetId="7" r:id="rId1"/>
+    <sheet name="HTTP Komunikace" sheetId="2" r:id="rId2"/>
+    <sheet name="List1" sheetId="8" r:id="rId3"/>
+    <sheet name="Dynamické WiFi" sheetId="3" r:id="rId4"/>
+    <sheet name="Statické WiFi" sheetId="5" r:id="rId5"/>
+    <sheet name="Zabezpečení" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="42">
   <si>
     <t>[mAh]</t>
   </si>
@@ -125,6 +127,45 @@
   <si>
     <t>Kalibrace</t>
   </si>
+  <si>
+    <t>Platforma</t>
+  </si>
+  <si>
+    <t>Režim</t>
+  </si>
+  <si>
+    <t>snímková frekvence</t>
+  </si>
+  <si>
+    <t>Počet snímků</t>
+  </si>
+  <si>
+    <t>Doba odezvy</t>
+  </si>
+  <si>
+    <t>[fps]</t>
+  </si>
+  <si>
+    <t>[frames]</t>
+  </si>
+  <si>
+    <t>[ms]</t>
+  </si>
+  <si>
+    <t>ESP8266</t>
+  </si>
+  <si>
+    <t>Kontinuální</t>
+  </si>
+  <si>
+    <t>ESP32</t>
+  </si>
+  <si>
+    <t>Enable</t>
+  </si>
+  <si>
+    <t>Deep sleep</t>
+  </si>
 </sst>
 </file>
 
@@ -148,7 +189,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -291,11 +332,184 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -336,6 +550,47 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -855,10 +1110,170 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310434CE-6D04-4CB0-8F23-E3FFD5FE60A2}">
+  <dimension ref="B2:F9"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="28"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="22">
+        <v>240</v>
+      </c>
+      <c r="E4" s="23">
+        <v>47</v>
+      </c>
+      <c r="F4" s="24">
+        <f>E4/D4*1000</f>
+        <v>195.83333333333334</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="32"/>
+      <c r="D5" s="22">
+        <v>240</v>
+      </c>
+      <c r="E5" s="25">
+        <v>45</v>
+      </c>
+      <c r="F5" s="24">
+        <f t="shared" ref="F5:F9" si="0">E5/D5*1000</f>
+        <v>187.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="22">
+        <v>240</v>
+      </c>
+      <c r="E6" s="23">
+        <v>770</v>
+      </c>
+      <c r="F6" s="24">
+        <f t="shared" si="0"/>
+        <v>3208.3333333333335</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="32"/>
+      <c r="D7" s="22">
+        <v>240</v>
+      </c>
+      <c r="E7" s="25">
+        <v>560</v>
+      </c>
+      <c r="F7" s="24">
+        <f t="shared" si="0"/>
+        <v>2333.3333333333335</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="22">
+        <v>240</v>
+      </c>
+      <c r="E8" s="23">
+        <v>236</v>
+      </c>
+      <c r="F8" s="24">
+        <f t="shared" si="0"/>
+        <v>983.33333333333326</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="32"/>
+      <c r="D9" s="22">
+        <v>240</v>
+      </c>
+      <c r="E9" s="23">
+        <v>257</v>
+      </c>
+      <c r="F9" s="24">
+        <f t="shared" si="0"/>
+        <v>1070.8333333333333</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0384769D-AB4F-4BE1-B26A-15ED3A0BBAB2}">
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
@@ -910,21 +1325,21 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="17" t="s">
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="19"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="36"/>
     </row>
     <row r="6" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E6" s="1" t="s">
@@ -1664,7 +2079,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7821DD-8698-4A0E-A4A3-BA7700C4ED5D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A851E2-6059-4EBB-B09A-8B0C3576633C}">
   <dimension ref="A1:O856"/>
   <sheetViews>
@@ -1717,21 +2144,21 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="17" t="s">
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="19"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="36"/>
     </row>
     <row r="6" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E6" s="1" t="s">
@@ -8651,7 +9078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26D2FC4-FCBF-4567-B8D1-6CD68584EE39}">
   <dimension ref="A2:O511"/>
   <sheetViews>
@@ -8699,21 +9126,21 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="17" t="s">
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="19"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="36"/>
     </row>
     <row r="6" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E6" s="1" t="s">
@@ -12876,7 +13303,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C320250A-50C6-4196-B533-B8E6EDBC8E7E}">
   <dimension ref="A1:O745"/>
   <sheetViews>
@@ -12931,21 +13358,21 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="17" t="s">
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="19"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="36"/>
     </row>
     <row r="6" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E6" s="1" t="s">

</xml_diff>